<commit_message>
Finished the constraint randomization according to the verification plan and also finished the FIFO_sequences achieving 100% code coverage
</commit_message>
<xml_diff>
--- a/verification plan/verification plan.xlsx
+++ b/verification plan/verification plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Shared Folders\Uni\courses\Digital circuit\digital github codes\Done\FIFO- UVM\verification plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Shared Folders\Uni\courses\Digital circuit\digital github codes\Done\FIFO -- UVM\FIFO--UVM\verification plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB16DDE0-B226-4037-9B51-248A85E47561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC795B0-93DC-4D9D-896D-99A85C2A8CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BE33C207-AC50-49BB-BEDD-1F59C983F64D}"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="28770" windowHeight="15450" xr2:uid="{BE33C207-AC50-49BB-BEDD-1F59C983F64D}"/>
   </bookViews>
   <sheets>
     <sheet name="Verification Plan" sheetId="1" r:id="rId1"/>
@@ -1039,8 +1039,8 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>

</xml_diff>

<commit_message>
Updated the functional coverage of the FIFO
</commit_message>
<xml_diff>
--- a/verification plan/verification plan.xlsx
+++ b/verification plan/verification plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Shared Folders\Uni\courses\Digital circuit\digital github codes\Done\FIFO -- UVM\FIFO--UVM\verification plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC795B0-93DC-4D9D-896D-99A85C2A8CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5EFC0D-8EB7-43E7-A2C9-8487F95DA704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="30" windowWidth="28770" windowHeight="15450" xr2:uid="{BE33C207-AC50-49BB-BEDD-1F59C983F64D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="103">
   <si>
     <t>#</t>
   </si>
@@ -196,9 +196,6 @@
 Coverpoint: FIFO_cov_grp::empty_cp</t>
   </si>
   <si>
-    <t>Cross: FIFO_cov_grp::wr_ack_empty_cr</t>
-  </si>
-  <si>
     <t>Ensure that the FIFO flags outputs matches the golden model flags outputs under randomized inputs
 Verify that data_out of the FIFO matches the data_out of the golden model</t>
   </si>
@@ -213,13 +210,6 @@
   </si>
   <si>
     <t>Write Opertaion when almost empty</t>
-  </si>
-  <si>
-    <t>Cross: FIFO_cov_grp::wr_ack_almostempty_cr</t>
-  </si>
-  <si>
-    <t>Cross: FIFO_cov_grp::wr_en_almostfull_cr
-Cross: FIFO_cov_grp::wr_ack_almost_full_cr</t>
   </si>
   <si>
     <t>Assertion: assert_wr_en_high
@@ -244,12 +234,6 @@
     <t>Ensure a successful write operation when FIFO is almost full.</t>
   </si>
   <si>
-    <t>Cross: FIFO_cov_grp::wr_ack_full_cr
-Cross: FIFO_cov_grp::full_almostfull_cr
-Cross: FIFO_cov_grp::wr_en_overflow_cr
-Cross: FIFO_cov_grp::full_overflow_cr</t>
-  </si>
-  <si>
     <t>Write Opertaion when full &amp; overflow</t>
   </si>
   <si>
@@ -284,20 +268,6 @@
   </si>
   <si>
     <t>Read Operation when empty &amp; underflow</t>
-  </si>
-  <si>
-    <t>Cross: FIFO_cov_grp::rd_en_almostfull_cr</t>
-  </si>
-  <si>
-    <t>Cross: FIFO_cov_grp::rd_en_full_cr</t>
-  </si>
-  <si>
-    <t>Cross: FIFO_cov_grp::rd_en_almostempty_cr</t>
-  </si>
-  <si>
-    <t>Cross: FIFO_cov_grp::rd_en_underflow_cr
-Cross: FIFO_cov_grp::empty_underflow_cr
-Cross: FIFO_cov_grp::empty_almostempty_cr</t>
   </si>
   <si>
     <t>Coverpoint: FIFO_cov_grp::rd_en_cp
@@ -368,6 +338,36 @@
   </si>
   <si>
     <t>Equal distribution probability to both read and write operations of becoming HIGH</t>
+  </si>
+  <si>
+    <t>Cross: FIFO_cov_grp::wr_ack_almostfull_wr_en_cr</t>
+  </si>
+  <si>
+    <t>Cross: FIFO_cov_grp::wr_ack_almostempty_wr_en_cr</t>
+  </si>
+  <si>
+    <t>Cross: FIFO_cov_grp::wr_ack_empty_wr_en_cr</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Cross: FIFO_cov_grp::wr_ack_full_wr_en_cr
+Cross: FIFO_cov_grp::full_almostfull_cr
+Cross: FIFO_cov_grp::overflow_cr</t>
+  </si>
+  <si>
+    <t>Cross: FIFO_cov_grp::underflow_cr
+Cross: FIFO_cov_grp::empty_almostempty_cr</t>
+  </si>
+  <si>
+    <t>Cross: FIFO_cov_grp::almostfull_rd_en_cr</t>
+  </si>
+  <si>
+    <t>Cross: FIFO_cov_grp::almostempty_rd_en_cr</t>
+  </si>
+  <si>
+    <t>Cross: FIFO_cov_grp::full_rd_en_cr</t>
   </si>
 </sst>
 </file>
@@ -1038,9 +1038,9 @@
   </sheetPr>
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -1048,7 +1048,7 @@
     <col min="1" max="1" width="8" style="8" customWidth="1"/>
     <col min="2" max="2" width="57" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="69.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62" style="7" customWidth="1"/>
+    <col min="4" max="4" width="66.7109375" style="7" customWidth="1"/>
     <col min="5" max="5" width="38.42578125" style="8" customWidth="1"/>
     <col min="6" max="6" width="61.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="8" customWidth="1"/>
@@ -1175,10 +1175,10 @@
         <v>43</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -1206,10 +1206,10 @@
         <v>48</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G6" s="3">
         <v>1</v>
@@ -1236,10 +1236,10 @@
         <v>47</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
@@ -1266,10 +1266,10 @@
         <v>46</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="G8" s="3">
         <v>1</v>
@@ -1296,10 +1296,10 @@
         <v>45</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="G9" s="3">
         <v>1</v>
@@ -1326,10 +1326,10 @@
         <v>44</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="G10" s="3">
         <v>1</v>
@@ -1389,7 +1389,7 @@
         <v>8</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="G12" s="3">
         <v>1</v>
@@ -1419,7 +1419,7 @@
         <v>8</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="G13" s="3">
         <v>1</v>
@@ -1443,13 +1443,13 @@
         <v>36</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="G14" s="3">
         <v>1</v>
@@ -1473,13 +1473,13 @@
         <v>35</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="G15" s="3">
         <v>1</v>
@@ -1524,22 +1524,22 @@
     </row>
     <row r="17" spans="1:10" ht="36">
       <c r="A17" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>52</v>
-      </c>
       <c r="C17" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="G17" s="3">
         <v>1</v>
@@ -1548,28 +1548,28 @@
         <v>100</v>
       </c>
       <c r="I17" s="22" t="s">
-        <v>15</v>
+        <v>97</v>
       </c>
       <c r="J17" s="20"/>
     </row>
     <row r="18" spans="1:10" ht="36">
       <c r="A18" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="G18" s="3">
         <v>2</v>
@@ -1578,58 +1578,58 @@
         <v>100</v>
       </c>
       <c r="I18" s="22" t="s">
-        <v>15</v>
+        <v>97</v>
       </c>
       <c r="J18" s="20"/>
     </row>
     <row r="19" spans="1:10" ht="36">
       <c r="A19" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" s="3">
+        <v>1</v>
+      </c>
+      <c r="H19" s="5">
+        <v>100</v>
+      </c>
+      <c r="I19" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="J19" s="20"/>
+    </row>
+    <row r="20" spans="1:10" ht="54">
+      <c r="A20" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G19" s="3">
-        <v>1</v>
-      </c>
-      <c r="H19" s="5">
-        <v>100</v>
-      </c>
-      <c r="I19" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="J19" s="20"/>
-    </row>
-    <row r="20" spans="1:10" ht="72">
-      <c r="A20" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="C20" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="G20" s="3">
         <v>1</v>
@@ -1638,7 +1638,7 @@
         <v>100</v>
       </c>
       <c r="I20" s="22" t="s">
-        <v>15</v>
+        <v>97</v>
       </c>
       <c r="J20" s="20"/>
     </row>
@@ -1674,22 +1674,22 @@
     </row>
     <row r="22" spans="1:10" ht="36">
       <c r="A22" s="3" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>8</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="G22" s="3">
         <v>1</v>
@@ -1698,28 +1698,28 @@
         <v>100</v>
       </c>
       <c r="I22" s="22" t="s">
-        <v>15</v>
+        <v>97</v>
       </c>
       <c r="J22" s="20"/>
     </row>
-    <row r="23" spans="1:10" ht="54">
+    <row r="23" spans="1:10" ht="36">
       <c r="A23" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="G23" s="3">
         <v>1</v>
@@ -1728,28 +1728,28 @@
         <v>100</v>
       </c>
       <c r="I23" s="22" t="s">
-        <v>15</v>
+        <v>97</v>
       </c>
       <c r="J23" s="20"/>
     </row>
     <row r="24" spans="1:10" ht="36">
       <c r="A24" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="G24" s="3">
         <v>1</v>
@@ -1758,28 +1758,28 @@
         <v>100</v>
       </c>
       <c r="I24" s="22" t="s">
-        <v>15</v>
+        <v>97</v>
       </c>
       <c r="J24" s="20"/>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="3" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="G25" s="3">
         <v>2</v>
@@ -1788,28 +1788,28 @@
         <v>100</v>
       </c>
       <c r="I25" s="22" t="s">
-        <v>15</v>
+        <v>97</v>
       </c>
       <c r="J25" s="20"/>
     </row>
-    <row r="26" spans="1:10" ht="90">
+    <row r="26" spans="1:10" ht="72">
       <c r="A26" s="3">
         <v>3.7</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="G26" s="3">
         <v>1</v>

</xml_diff>

<commit_message>
Finished the functional verification of the synchronous FIFO with 100% code and functional coverage. Successfully completed all verification plan goals.
</commit_message>
<xml_diff>
--- a/verification plan/verification plan.xlsx
+++ b/verification plan/verification plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Shared Folders\Uni\courses\Digital circuit\digital github codes\Done\FIFO -- UVM\FIFO--UVM\verification plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5EFC0D-8EB7-43E7-A2C9-8487F95DA704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC57015-6378-4365-9540-65EC032188A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="30" windowWidth="28770" windowHeight="15450" xr2:uid="{BE33C207-AC50-49BB-BEDD-1F59C983F64D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="100">
   <si>
     <t>#</t>
   </si>
@@ -84,12 +84,6 @@
 empty.</t>
   </si>
   <si>
-    <t>Concurrent assertion to check for the asynchronous reset functionality</t>
-  </si>
-  <si>
-    <t>Pending</t>
-  </si>
-  <si>
     <t>FIFO empty</t>
   </si>
   <si>
@@ -126,18 +120,9 @@
     <t>FIFO almost empty</t>
   </si>
   <si>
-    <t>Verify when the FIFO has only one more read operation can be performed before the FIFO goes to empty, the almost empty flag is asserted</t>
-  </si>
-  <si>
     <t>Read &amp; Write Operation</t>
   </si>
   <si>
-    <t>Ensure that when a read and write enables are HIGH and the FIFO is empty, only writing will take place</t>
-  </si>
-  <si>
-    <t>Ensure that when a read and write enables are HIGH and the FIFO is full, only reading will take place</t>
-  </si>
-  <si>
     <t>Priority to Read Operation</t>
   </si>
   <si>
@@ -145,12 +130,6 @@
   </si>
   <si>
     <t>Write Operation</t>
-  </si>
-  <si>
-    <t>Verify that when write enable and full flag are active and read enable and empty flag are deasserted the write acknowledge will be LOW after one clock cycle</t>
-  </si>
-  <si>
-    <t>Verify that when the write enable is active and read enable, full and empty are deasserted the write acknowledge gets HIGH after one clock cycle</t>
   </si>
   <si>
     <t>Write Acknowledge is asserted</t>
@@ -194,10 +173,6 @@
   <si>
     <t>Assertion: assert_empty
 Coverpoint: FIFO_cov_grp::empty_cp</t>
-  </si>
-  <si>
-    <t>Ensure that the FIFO flags outputs matches the golden model flags outputs under randomized inputs
-Verify that data_out of the FIFO matches the data_out of the golden model</t>
   </si>
   <si>
     <t>3.5.1</t>
@@ -222,9 +197,6 @@
 Cross: FIFO_cov_grp::wr_en_w_ack_cr</t>
   </si>
   <si>
-    <t>Ensure an ignored write operation when FIFO is full..</t>
-  </si>
-  <si>
     <t>Ensure a successful write operation when FIFO is almost empty.</t>
   </si>
   <si>
@@ -246,9 +218,6 @@
     <t>3.5.4</t>
   </si>
   <si>
-    <t>Ensure a successful read operation when FIFO is almost full</t>
-  </si>
-  <si>
     <t>Read Operation when almostfull</t>
   </si>
   <si>
@@ -258,24 +227,12 @@
     <t>Read Opertaion when full</t>
   </si>
   <si>
-    <t>Ensure a successful read operation when FIFO is full</t>
-  </si>
-  <si>
-    <t>Ensure a successful read operation when FIFO is almost empty</t>
-  </si>
-  <si>
     <t>Ensure an ignored read operation when FIFO is empty.</t>
   </si>
   <si>
     <t>Read Operation when empty &amp; underflow</t>
   </si>
   <si>
-    <t>Coverpoint: FIFO_cov_grp::rd_en_cp
-Coverpoint: FIFO_cov_grp::data_out_cp
-Cross: FIFO_cov_grp::rd_en_data_out_cr
-Cross: FIFO_cov_grp::rd_en_wr_en_data_out_cr</t>
-  </si>
-  <si>
     <t>3.6.1</t>
   </si>
   <si>
@@ -289,55 +246,6 @@
   </si>
   <si>
     <t>Synchronous FIFO</t>
-  </si>
-  <si>
-    <t>Concurrent assertion to check for the FIFO empty flag</t>
-  </si>
-  <si>
-    <t>Concurrent assertion to check for the FIFO almost full flag</t>
-  </si>
-  <si>
-    <t>Concurrent assertion to check for the FIFO overflow flag</t>
-  </si>
-  <si>
-    <t>Concurrent assertion to check for the FIFO underflow flag</t>
-  </si>
-  <si>
-    <t>Concurrent assertion to check for the FIFO almost flag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Concurrent assertion to check for the FIFO full flag
-</t>
-  </si>
-  <si>
-    <t>Concurrent assertion to check for the write acknowledge, read pointer and data out</t>
-  </si>
-  <si>
-    <t>Concurrent assertion to check for the write acknowledge</t>
-  </si>
-  <si>
-    <t>FIFO outputs checked against golden model</t>
-  </si>
-  <si>
-    <t>Constrained Randomization to allow only write operations</t>
-  </si>
-  <si>
-    <t>Constrained Randomization to allow only read operations</t>
-  </si>
-  <si>
-    <t>Constrained Randomization to make wr_en has higher probability than rd_en of becoming HIGH</t>
-  </si>
-  <si>
-    <t>Constrained Randomization to make rd_en has higher probability than wr_en of becoming HIGH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Constrained Randomization to make rd_en has higher probability than wr_en of becoming HIGH </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Constrained Randomization to make wr_en has higher probability than rd_en of becoming HIGH </t>
-  </si>
-  <si>
-    <t>Equal distribution probability to both read and write operations of becoming HIGH</t>
   </si>
   <si>
     <t>Cross: FIFO_cov_grp::wr_ack_almostfull_wr_en_cr</t>
@@ -368,6 +276,87 @@
   </si>
   <si>
     <t>Cross: FIFO_cov_grp::full_rd_en_cr</t>
+  </si>
+  <si>
+    <t>Coverpoint: FIFO_cov_grp::rd_en_cp
+Coverpoint: FIFO_cov_grp::data_out_cp
+Cross: FIFO_cov_grp::rd_en_wr_en_data_out_cr</t>
+  </si>
+  <si>
+    <t>Ensure a successful read operation when FIFO is almost full.</t>
+  </si>
+  <si>
+    <t>Ensure that the FIFO flags outputs matches the golden model flags outputs under randomized inputs
+Verify that data_out of the FIFO matches the data_out of the golden model.</t>
+  </si>
+  <si>
+    <t>Ensure a successful read operation when FIFO is full.</t>
+  </si>
+  <si>
+    <t>Ensure a successful read operation when FIFO is almost empty.</t>
+  </si>
+  <si>
+    <t>Ensure an ignored write operation when FIFO is full.</t>
+  </si>
+  <si>
+    <t>Verify that when write enable and full flag, the write acknowledge will be LOW after one clock cycle.</t>
+  </si>
+  <si>
+    <t>Verify that when the write enable is active and full is deasserted the write acknowledge gets HIGH after one clock cycle.</t>
+  </si>
+  <si>
+    <t>Ensure that when a read and write enables are HIGH and the FIFO is full, only reading will take place.</t>
+  </si>
+  <si>
+    <t>Ensure that when a read and write enables are HIGH and the FIFO is empty, only writing will take place.</t>
+  </si>
+  <si>
+    <t>Verify when the FIFO has only one more read operation can be performed before the FIFO goes to empty, the almost empty flag is asserted.</t>
+  </si>
+  <si>
+    <t>Equal distribution probability to both read and write operations of becoming HIGH.</t>
+  </si>
+  <si>
+    <t>Constrained Randomization to allow only read operations.</t>
+  </si>
+  <si>
+    <t>Constrained Randomization to allow only write operations.</t>
+  </si>
+  <si>
+    <t>Constrained Randomization to make rd_en has higher probability than wr_en of becoming HIGH.</t>
+  </si>
+  <si>
+    <t>Constrained Randomization to make wr_en has higher probability than rd_en of becoming HIGH.</t>
+  </si>
+  <si>
+    <t>Concurrent assertion to check for the asynchronous reset functionality.</t>
+  </si>
+  <si>
+    <t>Concurrent assertion to check for the FIFO full flag.</t>
+  </si>
+  <si>
+    <t>Concurrent assertion to check for the FIFO empty flag.</t>
+  </si>
+  <si>
+    <t>Concurrent assertion to check for the FIFO almost full flag.</t>
+  </si>
+  <si>
+    <t>Concurrent assertion to check for the FIFO overflow flag.</t>
+  </si>
+  <si>
+    <t>Concurrent assertion to check for the FIFO underflow flag.</t>
+  </si>
+  <si>
+    <t>Concurrent assertion to check for the FIFO almost flag.</t>
+  </si>
+  <si>
+    <t>Concurrent assertion to check for the write acknowledge, read pointer and data out.</t>
+  </si>
+  <si>
+    <t>Concurrent assertion to check for the write acknowledge.</t>
+  </si>
+  <si>
+    <t>FIFO outputs checked against golden model.</t>
   </si>
 </sst>
 </file>
@@ -430,7 +419,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -454,19 +443,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -584,7 +560,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -638,7 +614,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -647,49 +629,40 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1038,9 +1011,9 @@
   </sheetPr>
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -1058,49 +1031,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="13" customFormat="1" ht="23.25" thickTop="1" thickBot="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="33" t="s">
+      <c r="B1" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="34" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:13" s="12" customFormat="1" ht="21" thickTop="1">
-      <c r="A2" s="27">
-        <v>1</v>
-      </c>
-      <c r="B2" s="28" t="s">
+      <c r="A2" s="26">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="30"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="29"/>
       <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:13" ht="144">
@@ -1114,13 +1087,13 @@
         <v>13</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="G3" s="3">
         <v>1</v>
@@ -1129,7 +1102,7 @@
         <v>100</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="J3" s="20"/>
     </row>
@@ -1138,7 +1111,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>8</v>
@@ -1166,19 +1139,19 @@
         <v>2.1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>89</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -1186,10 +1159,10 @@
       <c r="H5" s="5">
         <v>100</v>
       </c>
-      <c r="I5" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="24"/>
+      <c r="I5" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5" s="23"/>
       <c r="M5" s="9"/>
     </row>
     <row r="6" spans="1:13" ht="72">
@@ -1197,19 +1170,19 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="G6" s="3">
         <v>1</v>
@@ -1217,29 +1190,29 @@
       <c r="H6" s="5">
         <v>100</v>
       </c>
-      <c r="I6" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="24"/>
+      <c r="I6" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="J6" s="23"/>
     </row>
     <row r="7" spans="1:13" ht="72">
       <c r="A7" s="3">
         <v>2.2999999999999998</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>20</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>89</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
@@ -1247,29 +1220,29 @@
       <c r="H7" s="5">
         <v>100</v>
       </c>
-      <c r="I7" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="24"/>
+      <c r="I7" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" s="23"/>
     </row>
     <row r="8" spans="1:13" ht="72">
       <c r="A8" s="3">
         <v>2.4</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="D8" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="G8" s="3">
         <v>1</v>
@@ -1277,29 +1250,29 @@
       <c r="H8" s="5">
         <v>100</v>
       </c>
-      <c r="I8" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="24"/>
+      <c r="I8" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" s="23"/>
     </row>
     <row r="9" spans="1:13" ht="72">
       <c r="A9" s="3">
         <v>2.5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="G9" s="3">
         <v>1</v>
@@ -1307,29 +1280,29 @@
       <c r="H9" s="5">
         <v>100</v>
       </c>
-      <c r="I9" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="24"/>
+      <c r="I9" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="23"/>
     </row>
     <row r="10" spans="1:13" ht="72">
       <c r="A10" s="3">
         <v>2.6</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="G10" s="3">
         <v>1</v>
@@ -1337,17 +1310,17 @@
       <c r="H10" s="5">
         <v>100</v>
       </c>
-      <c r="I10" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="24"/>
+      <c r="I10" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10" s="23"/>
     </row>
     <row r="11" spans="1:13" s="12" customFormat="1" ht="20.25">
       <c r="A11" s="1">
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>8</v>
@@ -1367,7 +1340,7 @@
       <c r="H11" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="25" t="s">
+      <c r="I11" s="24" t="s">
         <v>8</v>
       </c>
       <c r="J11" s="19"/>
@@ -1377,19 +1350,19 @@
         <v>3.1</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="E12" s="10" t="s">
         <v>8</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="G12" s="3">
         <v>1</v>
@@ -1398,7 +1371,7 @@
         <v>100</v>
       </c>
       <c r="I12" s="22" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="J12" s="20"/>
     </row>
@@ -1407,19 +1380,19 @@
         <v>3.2</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>8</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="G13" s="3">
         <v>1</v>
@@ -1428,7 +1401,7 @@
         <v>100</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="J13" s="20"/>
     </row>
@@ -1437,19 +1410,19 @@
         <v>3.3</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>87</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="G14" s="3">
         <v>1</v>
@@ -1458,7 +1431,7 @@
         <v>100</v>
       </c>
       <c r="I14" s="22" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="J14" s="20"/>
     </row>
@@ -1467,19 +1440,19 @@
         <v>3.4</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>87</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="G15" s="3">
         <v>1</v>
@@ -1488,7 +1461,7 @@
         <v>100</v>
       </c>
       <c r="I15" s="22" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="J15" s="20"/>
     </row>
@@ -1497,7 +1470,7 @@
         <v>3.5</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>8</v>
@@ -1517,29 +1490,29 @@
       <c r="H16" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="26" t="s">
+      <c r="I16" s="25" t="s">
         <v>8</v>
       </c>
       <c r="J16" s="19"/>
     </row>
     <row r="17" spans="1:10" ht="36">
       <c r="A17" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>59</v>
-      </c>
       <c r="D17" s="7" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>87</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="G17" s="3">
         <v>1</v>
@@ -1548,28 +1521,28 @@
         <v>100</v>
       </c>
       <c r="I17" s="22" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="J17" s="20"/>
     </row>
     <row r="18" spans="1:10" ht="36">
       <c r="A18" s="8" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>87</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="G18" s="3">
         <v>2</v>
@@ -1578,28 +1551,28 @@
         <v>100</v>
       </c>
       <c r="I18" s="22" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="J18" s="20"/>
     </row>
     <row r="19" spans="1:10" ht="36">
       <c r="A19" s="3" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>87</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="G19" s="3">
         <v>1</v>
@@ -1608,28 +1581,28 @@
         <v>100</v>
       </c>
       <c r="I19" s="22" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="J19" s="20"/>
     </row>
     <row r="20" spans="1:10" ht="54">
       <c r="A20" s="8" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>87</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="G20" s="3">
         <v>1</v>
@@ -1638,7 +1611,7 @@
         <v>100</v>
       </c>
       <c r="I20" s="22" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="J20" s="20"/>
     </row>
@@ -1647,7 +1620,7 @@
         <v>3.6</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>8</v>
@@ -1667,29 +1640,29 @@
       <c r="H21" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="I21" s="26" t="s">
+      <c r="I21" s="25" t="s">
         <v>8</v>
       </c>
       <c r="J21" s="19"/>
     </row>
     <row r="22" spans="1:10" ht="36">
       <c r="A22" s="3" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>8</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="G22" s="3">
         <v>1</v>
@@ -1698,29 +1671,29 @@
         <v>100</v>
       </c>
       <c r="I22" s="22" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="J22" s="20"/>
     </row>
     <row r="23" spans="1:10" ht="36">
       <c r="A23" s="3" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="C23" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="E23" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>86</v>
-      </c>
       <c r="G23" s="3">
         <v>1</v>
       </c>
@@ -1728,28 +1701,28 @@
         <v>100</v>
       </c>
       <c r="I23" s="22" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="J23" s="20"/>
     </row>
     <row r="24" spans="1:10" ht="36">
       <c r="A24" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="G24" s="3">
         <v>1</v>
@@ -1758,28 +1731,28 @@
         <v>100</v>
       </c>
       <c r="I24" s="22" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="J24" s="20"/>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="3" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="G25" s="3">
         <v>2</v>
@@ -1788,7 +1761,7 @@
         <v>100</v>
       </c>
       <c r="I25" s="22" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="J25" s="20"/>
     </row>
@@ -1797,19 +1770,19 @@
         <v>3.7</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="G26" s="3">
         <v>1</v>
@@ -1818,7 +1791,7 @@
         <v>100</v>
       </c>
       <c r="I26" s="22" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="J26" s="20"/>
     </row>

</xml_diff>